<commit_message>
memoria hecha, pero tengo que ver si recoloco los comentarios
</commit_message>
<xml_diff>
--- a/P1/MedidasRedesPractica1.xlsx
+++ b/P1/MedidasRedesPractica1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Nombre y apellidos del alumno: </t>
   </si>
@@ -252,15 +252,6 @@
   </si>
   <si>
     <t xml:space="preserve">1074 (0.9991)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Añadir aquí el gráfico de la distribución de grados&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Añadir aquí el gráfico de la distribución de distancias&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nota: En Gephi, este gráfico corresponde al de la medida de centralidad de distancia no normalizada</t>
   </si>
 </sst>
 </file>
@@ -270,7 +261,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -325,14 +316,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -432,7 +415,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,14 +458,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -497,21 +472,100 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>250200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>124200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>383400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>56880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Imagen 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="250200" y="3448080"/>
+          <a:ext cx="5943240" cy="3809520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>857520</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>199800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>56520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Imagen 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6667560" y="1161720"/>
+          <a:ext cx="5943240" cy="3809520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.4898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -694,68 +748,13 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -764,5 +763,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>